<commit_message>
Added one more task
New task added for notifying customer once order is ready to be
collected from the counter
</commit_message>
<xml_diff>
--- a/docs/DevTask@QRCode.xlsx
+++ b/docs/DevTask@QRCode.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>S.No</t>
   </si>
@@ -130,9 +130,6 @@
     <t>After marking the order as complete , the status should change in "collectOrder" table</t>
   </si>
   <si>
-    <t>After the order is collected it should get removed from the pending order list as well as from the "collectOrder" table.</t>
-  </si>
-  <si>
     <t>Order status to be updated on the order confirmation page(auto-refresh along with a refresh button)</t>
   </si>
   <si>
@@ -163,13 +160,19 @@
   </si>
   <si>
     <t>Interceptor class for calling and retrieving the generated UCOID from Utility class and saving the value in Order Model.</t>
+  </si>
+  <si>
+    <t>After the order is collected it should get removed from the pending order ( by changing the status to complete)</t>
+  </si>
+  <si>
+    <t>On the customer My Account create a Order Collect History page ( similar to OOB Order History page) showing the current staus of the order i.e. Pending or Complete (ready to be collected from counter).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,13 +184,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -284,12 +280,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -351,7 +349,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -386,7 +384,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -595,10 +593,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,10 +621,10 @@
         <v>5</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>2</v>
@@ -635,7 +633,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -648,10 +646,10 @@
       <c r="C2" s="3">
         <v>0.5</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>41946</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <v>41946</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -661,7 +659,7 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -674,20 +672,20 @@
       <c r="C3" s="3">
         <v>1.5</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>41946</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>41946</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -700,20 +698,20 @@
       <c r="C4" s="3">
         <v>0.5</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>41946</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>41946</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -726,10 +724,10 @@
       <c r="C5" s="3">
         <v>0.5</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>41946</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>41946</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -739,7 +737,7 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="72" customHeight="1" x14ac:dyDescent="0.25">
@@ -752,10 +750,10 @@
       <c r="C6" s="3">
         <v>0.5</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>41947</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>41947</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -765,7 +763,7 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -778,10 +776,10 @@
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>41947</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>41948</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -791,7 +789,7 @@
         <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -804,20 +802,20 @@
       <c r="C8" s="3">
         <v>1.5</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>41948</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>41949</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -825,23 +823,23 @@
         <v>8</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>41949</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>41950</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="13"/>
+        <v>38</v>
+      </c>
+      <c r="G9" s="12"/>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -854,10 +852,10 @@
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>41950</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="11">
         <v>41953</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -867,7 +865,7 @@
         <v>14</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
@@ -880,20 +878,20 @@
       <c r="C11" s="3">
         <v>0.5</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>41950</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="11">
         <v>41950</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
         <v>43</v>
-      </c>
-      <c r="H11" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -906,14 +904,14 @@
       <c r="C12" s="3">
         <v>1.5</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="11">
         <v>41950</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="11">
         <v>41953</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="6" t="s">
         <v>28</v>
@@ -923,7 +921,7 @@
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="3">
@@ -942,20 +940,20 @@
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="3">
         <v>1.5</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>41954</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="11">
         <v>41955</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G14" s="6" t="s">
         <v>30</v>
@@ -971,14 +969,14 @@
       <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="11">
         <v>41955</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="11">
         <v>41956</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="5"/>
     </row>
@@ -992,14 +990,14 @@
       <c r="C16" s="3">
         <v>1.5</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>41954</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <v>41955</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>32</v>
@@ -1015,39 +1013,60 @@
       <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>41955</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="11">
         <v>41956</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="11">
+        <v>41956</v>
+      </c>
+      <c r="E18" s="11">
+        <v>41957</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="12">
-        <v>41956</v>
-      </c>
-      <c r="E18" s="12">
-        <v>41957</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>36</v>
-      </c>
+    </row>
+    <row r="19" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="4">
+        <v>2</v>
+      </c>
+      <c r="D19" s="13">
+        <v>41954</v>
+      </c>
+      <c r="E19" s="13">
+        <v>41955</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
UI integration development plan
Included UI integration development plan
</commit_message>
<xml_diff>
--- a/docs/DevTask@QRCode.xlsx
+++ b/docs/DevTask@QRCode.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
   <si>
     <t>S.No</t>
   </si>
@@ -166,6 +166,48 @@
   </si>
   <si>
     <t>On the customer My Account create a Order Collect History page ( similar to OOB Order History page) showing the current staus of the order i.e. Pending or Complete (ready to be collected from counter).</t>
+  </si>
+  <si>
+    <t>New Template creation : Impex for template, Content Slot Names, Content Slot for template (for both desktop and mobile)</t>
+  </si>
+  <si>
+    <t>Create Template Structure VM file</t>
+  </si>
+  <si>
+    <t>Create Template JSP, with HTML code integration(for both desktop and mobile)</t>
+  </si>
+  <si>
+    <t>Create CSROrderListComponent, CSROrderDetailsComponent in items.xml extending SimpleCMSComponent.</t>
+  </si>
+  <si>
+    <t>With System Update</t>
+  </si>
+  <si>
+    <t>Create impexes for page, content slots, content slots for page, components</t>
+  </si>
+  <si>
+    <t>Modify header.tag/jsp with the current UI(when HTML code is available)(for both desktop and mobile)</t>
+  </si>
+  <si>
+    <t>Create CSR Orders Page Controller with JSP(integration with UI)(for both desktop and mobile)</t>
+  </si>
+  <si>
+    <t>Use code from existing PickInStoreOrder controller.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Controller for CSR Orders List Component
+UI integration with CSR Orders List Page JSP(for both desktop and mobile)
+</t>
+  </si>
+  <si>
+    <t>Create CSR Order Details Component functionality for retrieving order and customer details through AJAX
+UI integration with CSR Order details Page JSP(when HTML code is available)(for both desktop and mobile)</t>
+  </si>
+  <si>
+    <t>Auto import of impexes during initialization</t>
+  </si>
+  <si>
+    <t>Add importing impexes methods as well as synchronize methods</t>
   </si>
 </sst>
 </file>
@@ -203,7 +245,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -250,11 +292,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,6 +363,35 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -593,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,6 +1065,9 @@
       <c r="G14" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="H14" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -983,7 +1090,7 @@
       </c>
       <c r="G15" s="5"/>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1009,7 +1116,7 @@
         <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1032,6 +1139,9 @@
         <v>38</v>
       </c>
       <c r="G17" s="5"/>
+      <c r="H17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1055,6 +1165,9 @@
       <c r="G18" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="H18" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
@@ -1077,12 +1190,216 @@
       </c>
       <c r="G19" s="7"/>
       <c r="H19" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="14">
+        <v>1</v>
+      </c>
+      <c r="D20" s="23">
+        <v>41963</v>
+      </c>
+      <c r="E20" s="23">
+        <v>41963</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="16"/>
+    </row>
+    <row r="23" spans="1:8" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="18">
+        <v>41963</v>
+      </c>
+      <c r="E23" s="18">
+        <v>41963</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="18">
+        <v>41963</v>
+      </c>
+      <c r="E24" s="18">
+        <v>41963</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="16"/>
+    </row>
+    <row r="25" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="18">
+        <v>41963</v>
+      </c>
+      <c r="E25" s="18">
+        <v>41963</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="16"/>
+    </row>
+    <row r="26" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="15">
+        <v>1</v>
+      </c>
+      <c r="D26" s="18">
+        <v>41964</v>
+      </c>
+      <c r="E26" s="18">
+        <v>41964</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="D27" s="18">
+        <v>41963</v>
+      </c>
+      <c r="E27" s="18">
+        <v>41964</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="D28" s="18">
+        <v>41964</v>
+      </c>
+      <c r="E28" s="18">
+        <v>41967</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="16"/>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="20">
+        <v>1.5</v>
+      </c>
+      <c r="D29" s="18">
+        <v>41964</v>
+      </c>
+      <c r="E29" s="18">
+        <v>41967</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="21" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="5">
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new task and updated status
</commit_message>
<xml_diff>
--- a/docs/DevTask@QRCode.xlsx
+++ b/docs/DevTask@QRCode.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t>S.No</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t xml:space="preserve">This is done to add users in pending CSR queue based on beacon id and hence it will remove the hard coded dependency on uuid which was previously assumed to be unique user id. </t>
+  </si>
+  <si>
+    <t>Change comments on the order confirmation page and Order History Page</t>
+  </si>
+  <si>
+    <t>Add the comments - "Kindly collect your order from Aisle 10"</t>
   </si>
 </sst>
 </file>
@@ -410,15 +416,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,7 +486,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -515,7 +521,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -724,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,7 +795,7 @@
       <c r="G2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -815,7 +821,7 @@
       <c r="G3" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -841,7 +847,7 @@
       <c r="G4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -867,7 +873,7 @@
       <c r="G5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -893,7 +899,7 @@
       <c r="G6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -919,7 +925,7 @@
       <c r="G7" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -942,10 +948,10 @@
       <c r="F8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -968,8 +974,8 @@
       <c r="F9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="25" t="s">
+      <c r="G9" s="27"/>
+      <c r="H9" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -995,7 +1001,7 @@
       <c r="G10" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1021,7 +1027,7 @@
       <c r="G11" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1047,7 +1053,7 @@
       <c r="G12" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1069,7 +1075,7 @@
       <c r="G13" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="25"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
@@ -1093,7 +1099,7 @@
       <c r="G14" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="25" t="s">
+      <c r="H14" s="24" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1117,7 +1123,7 @@
         <v>39</v>
       </c>
       <c r="G15" s="20"/>
-      <c r="H15" s="25" t="s">
+      <c r="H15" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1143,7 +1149,7 @@
       <c r="G16" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1167,7 +1173,7 @@
         <v>38</v>
       </c>
       <c r="G17" s="20"/>
-      <c r="H17" s="25" t="s">
+      <c r="H17" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1193,7 +1199,7 @@
       <c r="G18" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="25"/>
+      <c r="H18" s="24"/>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
@@ -1215,7 +1221,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="20"/>
-      <c r="H19" s="25" t="s">
+      <c r="H19" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1238,10 +1244,10 @@
       <c r="F20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="25" t="s">
+      <c r="H20" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1267,7 +1273,7 @@
       <c r="G21" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="25" t="s">
+      <c r="H21" s="24" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1293,8 +1299,8 @@
       <c r="G22" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="25" t="s">
-        <v>48</v>
+      <c r="H22" s="24" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1319,7 +1325,9 @@
       <c r="G23" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="H23" s="25"/>
+      <c r="H23" s="24" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="12">
@@ -1343,7 +1351,7 @@
       <c r="G24" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="25"/>
+      <c r="H24" s="24"/>
     </row>
     <row r="25" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="12">
@@ -1367,7 +1375,9 @@
       <c r="G25" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="H25" s="25"/>
+      <c r="H25" s="24" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="12">
@@ -1391,7 +1401,7 @@
       <c r="G26" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="H26" s="25"/>
+      <c r="H26" s="24"/>
     </row>
     <row r="27" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
@@ -1400,22 +1410,46 @@
       <c r="B27" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="12">
         <v>1</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="14">
         <v>41964</v>
       </c>
-      <c r="E27" s="11">
+      <c r="E27" s="14">
         <v>41967</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="27" t="s">
+      <c r="G27" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="H27" s="26"/>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D28" s="11">
+        <v>41968</v>
+      </c>
+      <c r="E28" s="11">
+        <v>41968</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="H28" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Updated tasks. Added new
</commit_message>
<xml_diff>
--- a/docs/DevTask@QRCode.xlsx
+++ b/docs/DevTask@QRCode.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="68">
   <si>
     <t>S.No</t>
   </si>
@@ -172,9 +172,6 @@
 Create same for mobile as well.</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Create functionality for retrieving orders based on Date and Time.</t>
   </si>
   <si>
@@ -191,13 +188,7 @@
     <t>Use createdTS attribute to compare. Integrate it with Time Search on ordersListPage.jsp</t>
   </si>
   <si>
-    <t>Modify back end functionality for retrieving order and customer details through AJAX.</t>
-  </si>
-  <si>
     <t>Create fragment JSPs for order details.(desktop and mobile)(JSON format)(for now basic UI as HTML code is not available for order details yet)</t>
-  </si>
-  <si>
-    <t>Data as per screenshots</t>
   </si>
   <si>
     <t>Create a Sound Notification when new order is placed on CSR Dashboard</t>
@@ -238,6 +229,28 @@
 2. If new orders are returned through the AJAX(30 sec time interval query) , then Add more divs for the new orders below the orders list
 3. Simultaneously play a notification sound
 4. Simultaneously Increase the count on the bell icon as per the number of orders</t>
+  </si>
+  <si>
+    <t>Integrate Order Details UI with the available HTML code</t>
+  </si>
+  <si>
+    <t>Integrate Customer Details for the order with the available HTML code</t>
+  </si>
+  <si>
+    <t>Kindly consider all points :
+1. All products in tabular format along with their images, quantities, unit price and total price
+2. Dropdown for changing the order status - Use the same functionality existing with the previous UI.
+3. Ignore the check boxes</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>1. Customer details along with their image
+2. Also show the recently viewed products (create JSP or tag of the existing corresponding component.jsp, and add the supporting code of the component controller in the new controller.)
+3. Also show the wishlist products (create JSP or tag of the existing corresponding component.jsp, and add the supporting code of the component controller in the new controller.)
+4. Ignore the Assist Button for now
+5. Also ignore the Shopping Trend for now</t>
   </si>
 </sst>
 </file>
@@ -313,28 +326,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -353,11 +344,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -366,9 +381,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -383,9 +395,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -401,30 +410,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,28 +768,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -777,25 +797,25 @@
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3">
         <v>0.5</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>41946</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>41946</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -803,25 +823,25 @@
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="3">
         <v>1.5</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>41946</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>41946</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -829,25 +849,25 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="3">
         <v>0.5</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>41946</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>41946</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -855,25 +875,25 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3">
         <v>0.5</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>41946</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>41946</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -881,25 +901,25 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3">
         <v>0.5</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>41947</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>41947</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="20" t="s">
         <v>41</v>
       </c>
     </row>
@@ -907,555 +927,576 @@
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="9">
         <v>41947</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>41948</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="3">
         <v>1.5</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="9">
         <v>41948</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>41949</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="12">
         <v>41949</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>41950</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="27"/>
-      <c r="H9" s="24" t="s">
+      <c r="G9" s="21"/>
+      <c r="H9" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="12">
         <v>41950</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>41953</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="3">
         <v>0.5</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <v>41950</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>41950</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="3">
         <v>1.5</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>41950</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>41953</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="21" t="s">
+      <c r="G12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="12" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="24"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="3">
         <v>1.5</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="12">
         <v>41954</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="12">
         <v>41955</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="F14" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="20" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="12">
         <v>41955</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="12">
         <v>41956</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="F15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G15" s="20"/>
-      <c r="H15" s="24" t="s">
+      <c r="G15" s="16"/>
+      <c r="H15" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="C16" s="3">
         <v>1.5</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="12">
         <v>41954</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="12">
         <v>41955</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="F16" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="12">
         <v>41955</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="12">
         <v>41956</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="24" t="s">
+      <c r="G17" s="16"/>
+      <c r="H17" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>45</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="12">
         <v>41956</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="12">
         <v>41957</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="24"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="10">
         <v>2</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="12">
         <v>41954</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="12">
         <v>41955</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="24" t="s">
+      <c r="G19" s="16"/>
+      <c r="H19" s="20" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="D20" s="12">
+        <v>41963</v>
+      </c>
+      <c r="E20" s="12">
+        <v>41963</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="12">
+      <c r="H20" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="10">
         <v>1</v>
       </c>
-      <c r="D20" s="14">
-        <v>41963</v>
-      </c>
-      <c r="E20" s="14">
-        <v>41963</v>
-      </c>
-      <c r="F20" s="12" t="s">
+      <c r="D21" s="12">
+        <v>41964</v>
+      </c>
+      <c r="E21" s="12">
+        <v>41964</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G20" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
-        <v>20</v>
-      </c>
-      <c r="B21" s="13" t="s">
+      <c r="G21" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="H21" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="10">
+        <v>1</v>
+      </c>
+      <c r="D22" s="12">
+        <v>41964</v>
+      </c>
+      <c r="E22" s="12">
+        <v>41964</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H22" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>22</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="10">
+        <v>1</v>
+      </c>
+      <c r="D23" s="12">
+        <v>41967</v>
+      </c>
+      <c r="E23" s="12">
+        <v>41967</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="12">
+      <c r="H23" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>23</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" s="10">
         <v>1</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D24" s="12">
+        <v>41968</v>
+      </c>
+      <c r="E24" s="12">
+        <v>41968</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>24</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="10">
+        <v>1</v>
+      </c>
+      <c r="D25" s="12">
+        <v>41968</v>
+      </c>
+      <c r="E25" s="12">
+        <v>41969</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>25</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="10">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12">
         <v>41964</v>
       </c>
-      <c r="E21" s="14">
-        <v>41964</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="21" t="s">
+      <c r="E26" s="12">
+        <v>41967</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G26" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
-        <v>21</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="12">
-        <v>1</v>
-      </c>
-      <c r="D22" s="14">
-        <v>41964</v>
-      </c>
-      <c r="E22" s="14">
-        <v>41964</v>
-      </c>
-      <c r="F22" s="12" t="s">
+      <c r="H26" s="20"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>26</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="25">
+        <v>41968</v>
+      </c>
+      <c r="E27" s="26">
+        <v>41968</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="20"/>
+    </row>
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>27</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="24">
+        <v>2</v>
+      </c>
+      <c r="D28" s="23">
+        <v>41968</v>
+      </c>
+      <c r="E28" s="27">
+        <v>41969</v>
+      </c>
+      <c r="F28" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="12">
-        <v>22</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="D23" s="14">
-        <v>41964</v>
-      </c>
-      <c r="E23" s="14">
-        <v>41967</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="12">
-        <v>23</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="12">
-        <v>1</v>
-      </c>
-      <c r="D24" s="14">
-        <v>41968</v>
-      </c>
-      <c r="E24" s="14">
-        <v>41968</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A25" s="12">
-        <v>24</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="12">
-        <v>1</v>
-      </c>
-      <c r="D25" s="14">
-        <v>41967</v>
-      </c>
-      <c r="E25" s="14">
-        <v>41967</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" s="16" t="s">
+      <c r="G28" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="H25" s="24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="12">
-        <v>25</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="12">
-        <v>1.5</v>
-      </c>
-      <c r="D26" s="14">
-        <v>41967</v>
-      </c>
-      <c r="E26" s="14">
-        <v>41968</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="H26" s="24"/>
-    </row>
-    <row r="27" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="17">
-        <v>26</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="12">
-        <v>1</v>
-      </c>
-      <c r="D27" s="14">
-        <v>41964</v>
-      </c>
-      <c r="E27" s="14">
-        <v>41967</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="24"/>
-    </row>
-    <row r="28" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D28" s="11">
-        <v>41969</v>
-      </c>
-      <c r="E28" s="11">
-        <v>41969</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="26" t="s">
+      <c r="H28" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>28</v>
+      </c>
+      <c r="B29" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="H28" s="25"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="H28:H29"/>
     <mergeCell ref="G8:G9"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added new tasks for Customers Dashboard UI Integration
Added new tasks for Customers Dashboard UI Integration
29-40
</commit_message>
<xml_diff>
--- a/docs/DevTask@QRCode.xlsx
+++ b/docs/DevTask@QRCode.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="90">
   <si>
     <t>S.No</t>
   </si>
@@ -240,14 +240,110 @@
 3. Ignore the check boxes</t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
     <t>1. Customer details along with their image
 2. Also show the recently viewed products (create JSP or tag of the existing corresponding component.jsp, and add the supporting code of the component controller in the new controller.)
 3. Also show the wishlist products (create JSP or tag of the existing corresponding component.jsp, and add the supporting code of the component controller in the new controller.)
 4. Ignore the Assist Button for now
 5. Also ignore the Shopping Trend for now</t>
+  </si>
+  <si>
+    <t>The chart has to be made as navigation, and their counts to be properly updated. 
+On their respective clicks, the status as per LoggedIn as Queued, InService as Active, Completed as Serviced to be shown
+Also, by default the first customer has to be shown  as selected and their details on the right panel.</t>
+  </si>
+  <si>
+    <t>Add Order history, Recommended Products, Recently Viewed Products and Wishlist on the customer details page
+Add JSPs from the components and as done previously for the customer details for orders dashboard with similar changes in controller.</t>
+  </si>
+  <si>
+    <t>Implement the Search functionality similar to the UCOID search in the orders dashboard. Search has to be based on Customer name.(AJAX Search)
+Also, the first customer should be shown as selected by default and his details on the right panel 
+Create methods for searching the CSRCustomerDetails table by customerName in Dao, Facade, Service, Controller.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement the Date Time Search similar to the one implemented for orders dashboard with new methods for the same in DAO, Services, Facades, Controllers.(AJAX Search)
+Also, the first customer should be shown as selected by default and his details on the right panel </t>
+  </si>
+  <si>
+    <t>1. On Serviced Tab, display the list of CSRCustomerDetailsModel which are in COMPLETED status.
+2. Also, show at the bottom of the Customer Name, "assisted by &lt;AGENT NAme&gt;"
+3. Show no button on the right panel.</t>
+  </si>
+  <si>
+    <t>1. On Active Tab, display the list of CSRCustomerDetailsModel which are InService status. 
+2. Also, show at the bottom of the Customer Name, "assisted by &lt;AGENT NAme&gt;"
+3. Show only Serviced Button on the right panel, and this button should be visible only to the CSR agent who is assisting the customer</t>
+  </si>
+  <si>
+    <t>Implement the functionality of Assist Button. On click of the button, the CSRStoreStatus of the CSRCustomerDetails should change to InService status.
+UI wise, check that the customer details are no longer shown on the Queued Page and should be shown on the Active Page.</t>
+  </si>
+  <si>
+    <t>Implement the functionality of Serviced Button. On click of the button, the CSRStoreStatus of the CSRCustomerDetails should change to Completed status.
+UI wise, check that the customer is no longer shown on the Active Page and should be shown on the Serviced Page</t>
+  </si>
+  <si>
+    <t>Implement Send Greeting functionality.
+1. A text window has to be shown on clicking the Send Greeting button.
+2. The text window should show some default Text, and must be editable by the CSR agent.
+3. On click of Send Button, an email should be sent to the customer on their email id.
+for now assume the email from id to be as csr@bncstore.com
+4. On click of cancel button the text window should close.</t>
+  </si>
+  <si>
+    <t>On click of customer names on the left panel, their corresponsing details should be opened on the right panel.
+Also show the customer name as selected on the left panel.</t>
+  </si>
+  <si>
+    <t>Customers Dashboard UI Integration as per personal_data.html with following changes(modify the customerDetailsPage.jsp):
+1. Add buttons - Send Greeting, Assist, No Thanks on the top as per send_greetings.html
+2. Show the top customer as selected by default with their details on right side
+3. Status monitoring to be done as per enumtype CSRStoreStatus, with LoggedIn as Queued, InService as Active, Completed as Serviced.
+4. The Queued page has to show the LoggedIn status customers for the day.
+5. Changes in methods in DAO, Services, Facades, Controllers as required.
+6. Create proper tags for the same instead of everything to be on one JSP.
+7. Remove dependency on template</t>
+  </si>
+  <si>
+    <t>Integrate new Customers Landing Page UI with existing code</t>
+  </si>
+  <si>
+    <t>Implement search by customer name functionality</t>
+  </si>
+  <si>
+    <t>Chart Navigation and their count to be made dynamic</t>
+  </si>
+  <si>
+    <t>Add Order history, Recommended Products, Recently Viewed Products and Wishlist on the customer details page</t>
+  </si>
+  <si>
+    <t>Implement the Date Time Search</t>
+  </si>
+  <si>
+    <t>The notification bell should show the count equal to number of queued customers.
+Page must be refreshed through AJAX every 60 seconds. 
+With every new addition of customer in queued list, a sound should be played.</t>
+  </si>
+  <si>
+    <t>The notification bell count and ajax refresh of queued customers</t>
+  </si>
+  <si>
+    <t>Implement the Active Page functionality</t>
+  </si>
+  <si>
+    <t>Implement the Serviced Page functionality</t>
+  </si>
+  <si>
+    <t>Implement the Assist Button functionality</t>
+  </si>
+  <si>
+    <t>Implement the Serviced Button functionality</t>
+  </si>
+  <si>
+    <t>Implement Send Greeting functionality.</t>
+  </si>
+  <si>
+    <t>On click of customer names on the left panel, their corresponsing details should be opened on the right panel.</t>
   </si>
 </sst>
 </file>
@@ -285,7 +381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -349,6 +445,19 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -358,18 +467,37 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1" tint="0.249977111117893"/>
+      </left>
+      <right style="thick">
+        <color theme="1" tint="0.249977111117893"/>
+      </right>
+      <top style="thick">
+        <color theme="1" tint="0.249977111117893"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -422,32 +550,49 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,7 +654,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -544,7 +689,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -753,10 +898,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -971,7 +1116,7 @@
       <c r="F8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="33" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="20" t="s">
@@ -997,7 +1142,7 @@
       <c r="F9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="25"/>
+      <c r="G9" s="33"/>
       <c r="H9" s="20" t="s">
         <v>41</v>
       </c>
@@ -1400,8 +1545,8 @@
       <c r="G25" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H25" s="23" t="s">
-        <v>65</v>
+      <c r="H25" s="20" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1460,44 +1605,333 @@
       <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="24">
+      <c r="C28" s="34">
         <v>2</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="36">
         <v>41968</v>
       </c>
-      <c r="E28" s="27">
+      <c r="E28" s="36">
         <v>41969</v>
       </c>
-      <c r="F28" s="29" t="s">
+      <c r="F28" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="14" t="s">
+      <c r="G28" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="H28" s="30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="H28" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="24"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="14" t="s">
+      <c r="C29" s="35"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="H29" s="32"/>
+    </row>
+    <row r="30" spans="1:8" ht="151.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="26">
+        <v>29</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" s="26">
+        <v>2</v>
+      </c>
+      <c r="D30" s="21">
+        <v>41981</v>
+      </c>
+      <c r="E30" s="21">
+        <v>41983</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H30" s="29"/>
+    </row>
+    <row r="31" spans="1:8" ht="76.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="26">
+        <v>30</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="D31" s="21">
+        <v>41981</v>
+      </c>
+      <c r="E31" s="21">
+        <v>41981</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="29"/>
+    </row>
+    <row r="32" spans="1:8" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26">
+        <v>31</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="D32" s="21">
+        <v>41981</v>
+      </c>
+      <c r="E32" s="21">
+        <v>41981</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="H29" s="30"/>
-    </row>
+      <c r="H32" s="29"/>
+    </row>
+    <row r="33" spans="1:8" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="26">
+        <v>32</v>
+      </c>
+      <c r="B33" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="26">
+        <v>1</v>
+      </c>
+      <c r="D33" s="21">
+        <v>41982</v>
+      </c>
+      <c r="E33" s="21">
+        <v>41982</v>
+      </c>
+      <c r="F33" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33" s="29"/>
+    </row>
+    <row r="34" spans="1:8" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="26">
+        <v>33</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="26">
+        <v>1</v>
+      </c>
+      <c r="D34" s="21">
+        <v>41983</v>
+      </c>
+      <c r="E34" s="21">
+        <v>41983</v>
+      </c>
+      <c r="F34" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="H34" s="29"/>
+    </row>
+    <row r="35" spans="1:8" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="26">
+        <v>34</v>
+      </c>
+      <c r="B35" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="D35" s="21">
+        <v>41984</v>
+      </c>
+      <c r="E35" s="21">
+        <v>41984</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="29"/>
+    </row>
+    <row r="36" spans="1:8" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="26">
+        <v>35</v>
+      </c>
+      <c r="B36" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="D36" s="21">
+        <v>41984</v>
+      </c>
+      <c r="E36" s="21">
+        <v>41984</v>
+      </c>
+      <c r="F36" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="H36" s="29"/>
+    </row>
+    <row r="37" spans="1:8" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="26">
+        <v>36</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="D37" s="21">
+        <v>41984</v>
+      </c>
+      <c r="E37" s="21">
+        <v>41984</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H37" s="29"/>
+    </row>
+    <row r="38" spans="1:8" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="26">
+        <v>37</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="D38" s="21">
+        <v>41984</v>
+      </c>
+      <c r="E38" s="21">
+        <v>41984</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="29"/>
+    </row>
+    <row r="39" spans="1:8" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="26">
+        <v>38</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="D39" s="21">
+        <v>41985</v>
+      </c>
+      <c r="E39" s="21">
+        <v>41985</v>
+      </c>
+      <c r="F39" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="H39" s="29"/>
+    </row>
+    <row r="40" spans="1:8" ht="91.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="26">
+        <v>39</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="26">
+        <v>1</v>
+      </c>
+      <c r="D40" s="21">
+        <v>41985</v>
+      </c>
+      <c r="E40" s="21">
+        <v>41985</v>
+      </c>
+      <c r="F40" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="H40" s="29"/>
+    </row>
+    <row r="41" spans="1:8" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="26">
+        <v>40</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" s="26">
+        <v>1</v>
+      </c>
+      <c r="D41" s="21">
+        <v>41985</v>
+      </c>
+      <c r="E41" s="21">
+        <v>41988</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G41" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="H41" s="29"/>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="H28:H29"/>

</xml_diff>